<commit_message>
Anexe los arreglos de vocales y consonantes y agregue las especificaciones del arreglo de las partidas
</commit_message>
<xml_diff>
--- a/Wordix-programa/estructurasDatosWordix.xlsx
+++ b/Wordix-programa/estructurasDatosWordix.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monic\Documents\TUDW - UNCOMA\1 Cuatrimestre\Intro. Programacion\TP final\Wordix\Wordix-programa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="EstructuraDatos"/>
+    <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
@@ -70,9 +75,6 @@
     <t>"partida"</t>
   </si>
   <si>
-    <t>"palabra</t>
-  </si>
-  <si>
     <t>"QUESO"</t>
   </si>
   <si>
@@ -127,9 +129,6 @@
     <t>"No adivino la palabra"</t>
   </si>
   <si>
-    <t>"Adivino la palabra en 2 intentos</t>
-  </si>
-  <si>
     <t>"Adivino la palabra en 1 intento"</t>
   </si>
   <si>
@@ -143,13 +142,120 @@
   </si>
   <si>
     <t>"Adivino la palabra en 2 intentos"</t>
+  </si>
+  <si>
+    <t>Tipo: Multidimensional. Indexado (los índices son numéricos) con arreglos asociativos</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena en cada posición un arreglo asociativo con claves String y valores String y Entero</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar cada una de las partidas jugadas con los datos relevantes de cada una</t>
+  </si>
+  <si>
+    <t>$coleccionVocales</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t>"E"</t>
+  </si>
+  <si>
+    <t>"I"</t>
+  </si>
+  <si>
+    <t>"O"</t>
+  </si>
+  <si>
+    <t>"U"</t>
+  </si>
+  <si>
+    <t>$coleccionConsonant1</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t>"D"</t>
+  </si>
+  <si>
+    <t>"F"</t>
+  </si>
+  <si>
+    <t>"G"</t>
+  </si>
+  <si>
+    <t>"H"</t>
+  </si>
+  <si>
+    <t>"J"</t>
+  </si>
+  <si>
+    <t>"K"</t>
+  </si>
+  <si>
+    <t>"L"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>"B"</t>
+  </si>
+  <si>
+    <t>$coleccionConsonant2</t>
+  </si>
+  <si>
+    <t>"N"</t>
+  </si>
+  <si>
+    <t>"P"</t>
+  </si>
+  <si>
+    <t>"Q"</t>
+  </si>
+  <si>
+    <t>"R"</t>
+  </si>
+  <si>
+    <t>"S"</t>
+  </si>
+  <si>
+    <t>"T"</t>
+  </si>
+  <si>
+    <t>"W"</t>
+  </si>
+  <si>
+    <t>"V"</t>
+  </si>
+  <si>
+    <t>"X"</t>
+  </si>
+  <si>
+    <t>"Y"</t>
+  </si>
+  <si>
+    <t>"Z"</t>
+  </si>
+  <si>
+    <t>Tipo: Los 3 arreglos anteriores son arreglos Indexados (los índices son numéricos)</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacenan datos de tipo String</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar vocales y letras del abecedario para sumar a los puntajes obtenidos en cada partida</t>
+  </si>
+  <si>
+    <t>"palabra"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +266,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -174,7 +280,7 @@
     <font>
       <i/>
       <sz val="10"/>
-      <color rgb="FF00b050"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -193,7 +299,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFd4d4d4"/>
+      <color rgb="FFD4D4D4"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
@@ -213,7 +319,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -254,60 +360,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -318,10 +437,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -359,71 +478,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,7 +570,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -474,11 +593,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -487,13 +606,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -503,7 +622,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -512,7 +631,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -521,7 +640,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -529,10 +648,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -603,25 +722,27 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="12" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="31.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="30.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="28.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="27.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +758,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -651,7 +772,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -681,7 +802,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -709,7 +830,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -723,7 +844,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -739,7 +860,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -755,7 +876,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -771,7 +892,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -787,7 +908,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -801,7 +922,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -815,7 +936,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -831,7 +952,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -847,7 +968,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -861,7 +982,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -899,7 +1020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -937,85 +1058,85 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="J17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="K17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="J18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
@@ -1051,45 +1172,45 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="E20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="H20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="K20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="L20" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1103,9 +1224,11 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1117,9 +1240,11 @@
       <c r="K22" s="2"/>
       <c r="L22" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1131,9 +1256,11 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="11"/>
       <c r="E24" s="2"/>
@@ -1145,9 +1272,11 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C25" s="11"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1159,7 +1288,7 @@
       <c r="K25" s="11"/>
       <c r="L25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1173,7 +1302,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1187,13 +1316,25 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>4</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="10"/>
@@ -1201,13 +1342,23 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="B29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="10"/>
@@ -1215,7 +1366,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1229,7 +1380,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1241,37 +1392,79 @@
       <c r="I31" s="10"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4">
+        <v>4</v>
+      </c>
+      <c r="G32" s="4">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4">
+        <v>6</v>
+      </c>
+      <c r="I32" s="4">
+        <v>7</v>
+      </c>
+      <c r="J32" s="4">
+        <v>8</v>
+      </c>
+      <c r="K32" s="4">
+        <v>9</v>
+      </c>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="B33" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1283,9 +1476,9 @@
       <c r="I34" s="10"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1297,37 +1490,82 @@
       <c r="I35" s="10"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="3"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="3"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4</v>
+      </c>
+      <c r="G36" s="4">
+        <v>5</v>
+      </c>
+      <c r="H36" s="4">
+        <v>6</v>
+      </c>
+      <c r="I36" s="4">
+        <v>7</v>
+      </c>
+      <c r="J36" s="4">
+        <v>8</v>
+      </c>
+      <c r="K36" s="4">
+        <v>9</v>
+      </c>
+      <c r="L36" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1341,11 +1579,11 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="B39" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1355,11 +1593,11 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="B40" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1369,11 +1607,12 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="B41" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="11"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1383,11 +1622,12 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>

</xml_diff>

<commit_message>
Anexé el arreglo estadistJugador
</commit_message>
<xml_diff>
--- a/Wordix-programa/estructurasDatosWordix.xlsx
+++ b/Wordix-programa/estructurasDatosWordix.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
   <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
@@ -250,13 +250,52 @@
   </si>
   <si>
     <t>"palabra"</t>
+  </si>
+  <si>
+    <t>"partidas"</t>
+  </si>
+  <si>
+    <t>"puntaje</t>
+  </si>
+  <si>
+    <t>"victorias"</t>
+  </si>
+  <si>
+    <t>"intento1"</t>
+  </si>
+  <si>
+    <t>"intento2"</t>
+  </si>
+  <si>
+    <t>"intento3"</t>
+  </si>
+  <si>
+    <t>"intento4"</t>
+  </si>
+  <si>
+    <t>"intento5"</t>
+  </si>
+  <si>
+    <t>"intento6"</t>
+  </si>
+  <si>
+    <t>Tipo: Arreglo asociativo</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena datos de tipo String y numericos</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: traer y guardar los datos de un jugador desde el arreglo de las Partidas y mostrar las estadisticas del jugador en pantalla</t>
+  </si>
+  <si>
+    <t>$estadistJugador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +348,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -413,6 +460,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,15 +771,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="12" customWidth="1"/>
     <col min="2" max="2" width="21" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.44140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5546875" style="13" bestFit="1" customWidth="1"/>
@@ -1226,7 +1277,7 @@
     </row>
     <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2"/>
@@ -1581,7 +1632,7 @@
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="2"/>
@@ -1637,7 +1688,96 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="14">
+        <v>3</v>
+      </c>
+      <c r="D46" s="14">
+        <f>6+10+12</f>
+        <v>28</v>
+      </c>
+      <c r="E46" s="14">
+        <v>3</v>
+      </c>
+      <c r="F46" s="14">
+        <v>0</v>
+      </c>
+      <c r="G46" s="14">
+        <v>0</v>
+      </c>
+      <c r="H46" s="14">
+        <v>1</v>
+      </c>
+      <c r="I46" s="14">
+        <v>1</v>
+      </c>
+      <c r="J46" s="14">
+        <v>0</v>
+      </c>
+      <c r="K46" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B47" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregué el arreglo estadistJugador
</commit_message>
<xml_diff>
--- a/Wordix-programa/estructurasDatosWordix.xlsx
+++ b/Wordix-programa/estructurasDatosWordix.xlsx
@@ -773,8 +773,8 @@
   </sheetPr>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Agregue el ultimo arreglo de palabras ya jugadas por un jugador
</commit_message>
<xml_diff>
--- a/Wordix-programa/estructurasDatosWordix.xlsx
+++ b/Wordix-programa/estructurasDatosWordix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monic\Documents\TUDW - UNCOMA\1 Cuatrimestre\Intro. Programacion\TP final\Wordix\Wordix-programa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monic\Documents\TUDW - UNCOMA\1 Cuatrimestre\Intro. Programacion\TrabajoIntegradorFinal\Wordix\Wordix-programa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
-  <si>
-    <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -63,12 +60,6 @@
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
   </si>
   <si>
-    <t>A continuación puede agregar el resto de las estructuras de datos</t>
-  </si>
-  <si>
-    <t>**** COMPLETAR ****</t>
-  </si>
-  <si>
     <t>$coleccionPartidas</t>
   </si>
   <si>
@@ -289,6 +280,30 @@
   </si>
   <si>
     <t>$estadistJugador</t>
+  </si>
+  <si>
+    <t>Colecciones utilizadas</t>
+  </si>
+  <si>
+    <t>$palabrasJugadas</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>CEJAS</t>
+  </si>
+  <si>
+    <t>Tipo: Arreglo indexado</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena datos de tipo String</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Guardar  las palabras jugadas por un jugador determinado</t>
+  </si>
+  <si>
+    <t>Se genera solo cuando se ejecuta la función que lo requiere. No se guarda</t>
   </si>
 </sst>
 </file>
@@ -771,10 +786,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +810,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -825,7 +840,7 @@
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -846,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -856,25 +871,25 @@
     <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -898,7 +913,7 @@
     <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -914,7 +929,7 @@
     <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -930,7 +945,7 @@
     <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -946,7 +961,7 @@
     <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -988,9 +1003,6 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1004,9 +1016,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1035,7 +1045,7 @@
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -1073,7 +1083,7 @@
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
@@ -1111,83 +1121,83 @@
     </row>
     <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="J17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="K17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="G18" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
@@ -1225,40 +1235,40 @@
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="H20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="K20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="L20" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1278,7 +1288,7 @@
     <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1294,7 +1304,7 @@
     <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1310,7 +1320,7 @@
     <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="11"/>
@@ -1326,7 +1336,7 @@
     <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="2"/>
@@ -1369,7 +1379,7 @@
     </row>
     <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4">
         <v>0</v>
@@ -1396,19 +1406,19 @@
     <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1447,7 +1457,7 @@
     </row>
     <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" s="4">
         <v>0</v>
@@ -1484,34 +1494,34 @@
     <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="G33" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="H33" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="I33" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="J33" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="K33" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="L33"/>
     </row>
@@ -1545,7 +1555,7 @@
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
@@ -1583,37 +1593,37 @@
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="F37" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="G37" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="H37" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="14" t="s">
+      <c r="J37" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="K37" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="L37" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1633,7 +1643,7 @@
     <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1647,7 +1657,7 @@
     <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1661,7 +1671,7 @@
     <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="2"/>
@@ -1676,7 +1686,7 @@
     <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C42" s="11"/>
       <c r="E42" s="2"/>
@@ -1688,93 +1698,151 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
+      <c r="B46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="14">
+      <c r="D46" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="14">
         <v>3</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D55" s="14">
         <f>6+10+12</f>
         <v>28</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E55" s="14">
         <v>3</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F55" s="14">
         <v>0</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G55" s="14">
         <v>0</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H55" s="14">
         <v>1</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I55" s="14">
         <v>1</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J55" s="14">
         <v>0</v>
       </c>
-      <c r="K46" s="14">
+      <c r="K55" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="16" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="G56" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="H56" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="I56" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="J56" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="K56" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I47" s="16" t="s">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="J47" s="16" t="s">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K47" s="16" t="s">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="13" t="s">
-        <v>88</v>
-      </c>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B62" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>